<commit_message>
Add convert money to vnd text
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/PhieuChiTemplate.xlsx
+++ b/src/main/resources/ExportTemplate/PhieuChiTemplate.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>PAYMENT SHEET / PHIẾU CHI</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>${amount}</t>
+  </si>
+  <si>
+    <t>${amountVND}</t>
   </si>
 </sst>
 </file>
@@ -629,7 +632,7 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -787,7 +790,9 @@
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="16"/>
+      <c r="B11" s="16" t="s">
+        <v>23</v>
+      </c>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>

</xml_diff>

<commit_message>
update template tam ung
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/PhieuChiTemplate.xlsx
+++ b/src/main/resources/ExportTemplate/PhieuChiTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\workspace\ael\src\main\resources\ExportTemplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Working\Projects\GitHub\ael\src\main\resources\ExportTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -103,6 +103,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.00;[Red]#,##0.00"/>
+  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -171,7 +174,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -208,11 +211,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -275,6 +287,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -631,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -746,44 +767,44 @@
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-    </row>
-    <row r="9" spans="1:10" s="11" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+    </row>
+    <row r="9" spans="1:10" s="11" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
     </row>
     <row r="10" spans="1:10" s="11" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="12"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="35"/>
       <c r="J10" s="12"/>
     </row>
     <row r="11" spans="1:10" s="11" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1057,7 +1078,7 @@
     <row r="40" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="41" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="13">
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="E15:G15"/>
     <mergeCell ref="H15:J15"/>
@@ -1069,6 +1090,8 @@
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="H14:J14"/>
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="B8:J9"/>
   </mergeCells>
   <pageMargins left="0.2" right="0.2" top="0" bottom="0" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
In phieu thu/phieu chi done
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/PhieuChiTemplate.xlsx
+++ b/src/main/resources/ExportTemplate/PhieuChiTemplate.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28680" windowHeight="12660"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17805" windowHeight="4200"/>
   </bookViews>
   <sheets>
     <sheet name="PHIEU  CHI " sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
-  <extLst/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>PAYMENT SHEET / PHIẾU CHI</t>
   </si>
@@ -96,13 +96,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6">
     <font>
       <sz val="10"/>
@@ -212,23 +206,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -237,9 +216,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -262,15 +238,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -278,42 +245,125 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Comma[0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Percent" xfId="4" builtinId="5"/>
-    <cellStyle name="Currency[0]" xfId="5" builtinId="7"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1857375</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1025" name="Picture 1" descr="logo-AEL.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="19050"/>
+          <a:ext cx="1857375" cy="619125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -611,6 +661,7 @@
           </a:gdLst>
           <a:ahLst/>
           <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst>
             <a:path w="21600" h="21600"/>
           </a:pathLst>
@@ -643,229 +694,228 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:J20"/>
+      <selection activeCell="I5" sqref="I5:J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="28" style="3" customWidth="1"/>
-    <col min="2" max="2" width="6.57142857142857" style="3" customWidth="1"/>
-    <col min="3" max="3" width="9.14285714285714" style="3"/>
-    <col min="4" max="4" width="10.7142857142857" style="3" customWidth="1"/>
-    <col min="5" max="5" width="4.57142857142857" style="3" customWidth="1"/>
-    <col min="6" max="6" width="11.4285714285714" style="3" customWidth="1"/>
-    <col min="7" max="7" width="6.57142857142857" style="3" customWidth="1"/>
-    <col min="8" max="8" width="8.42857142857143" style="3" customWidth="1"/>
-    <col min="9" max="9" width="9.14285714285714" style="3"/>
-    <col min="10" max="10" width="11.8571428571429" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="9.14285714285714" style="3"/>
+    <col min="2" max="2" width="6.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="3"/>
+    <col min="4" max="4" width="10.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="4.5703125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="3"/>
+    <col min="10" max="10" width="11.85546875" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.75" customHeight="1" spans="3:10">
-      <c r="C1" s="4" t="s">
+    <row r="1" spans="1:10" ht="12.75" customHeight="1">
+      <c r="C1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-    </row>
-    <row r="2" ht="12.75" customHeight="1" spans="2:10">
-      <c r="B2" s="5"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-    </row>
-    <row r="3" ht="12.75" customHeight="1" spans="3:10">
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-    </row>
-    <row r="4" ht="24" customHeight="1" spans="3:10">
-      <c r="C4" s="6" t="s">
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+    </row>
+    <row r="2" spans="1:10" ht="12.75" customHeight="1">
+      <c r="B2" s="4"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+    </row>
+    <row r="3" spans="1:10" ht="12.75" customHeight="1">
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+    </row>
+    <row r="4" spans="1:10" ht="24" customHeight="1">
+      <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="30" t="s">
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="31"/>
-    </row>
-    <row r="5" s="1" customFormat="1" ht="26.25" customHeight="1" spans="1:10">
-      <c r="A5" s="9" t="s">
+      <c r="J4" s="22"/>
+    </row>
+    <row r="5" spans="1:10" s="1" customFormat="1" ht="26.25" customHeight="1">
+      <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="12" t="s">
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="32" t="s">
+      <c r="I5" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="32"/>
-    </row>
-    <row r="6" s="1" customFormat="1" ht="27" customHeight="1" spans="1:10">
-      <c r="A6" s="6" t="s">
+      <c r="J5" s="23"/>
+    </row>
+    <row r="6" spans="1:10" s="1" customFormat="1" ht="27" customHeight="1">
+      <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10" t="s">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-    </row>
-    <row r="7" s="1" customFormat="1" ht="27" customHeight="1" spans="1:10">
-      <c r="A7" s="11"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-    </row>
-    <row r="8" s="1" customFormat="1" ht="27" customHeight="1" spans="1:10">
-      <c r="A8" s="6" t="s">
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+    </row>
+    <row r="7" spans="1:10" s="1" customFormat="1" ht="27" customHeight="1">
+      <c r="A7" s="10"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+    </row>
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="27" customHeight="1">
+      <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-    </row>
-    <row r="9" s="1" customFormat="1" ht="27" customHeight="1" spans="1:10">
-      <c r="A9" s="11"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-    </row>
-    <row r="10" s="1" customFormat="1" ht="27" customHeight="1" spans="1:10">
-      <c r="A10" s="6" t="s">
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+    </row>
+    <row r="9" spans="1:10" s="1" customFormat="1" ht="27" customHeight="1">
+      <c r="A9" s="10"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+    </row>
+    <row r="10" spans="1:10" s="1" customFormat="1" ht="27" customHeight="1">
+      <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="13"/>
-    </row>
-    <row r="11" s="1" customFormat="1" ht="27.75" customHeight="1" spans="1:10">
-      <c r="A11" s="6" t="s">
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="12"/>
+    </row>
+    <row r="11" spans="1:10" s="1" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-    </row>
-    <row r="12" s="1" customFormat="1" ht="27" customHeight="1" spans="1:10">
-      <c r="A12" s="20"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-    </row>
-    <row r="13" ht="28.5" customHeight="1" spans="1:9">
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+    </row>
+    <row r="12" spans="1:10" s="1" customFormat="1" ht="27" customHeight="1">
+      <c r="A12" s="16"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+    </row>
+    <row r="13" spans="1:10" ht="28.5" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23" t="s">
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="24" t="s">
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
-    </row>
-    <row r="15" s="2" customFormat="1" spans="1:10">
-      <c r="A15" s="26" t="s">
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+    </row>
+    <row r="15" spans="1:10" s="2" customFormat="1">
+      <c r="A15" s="20" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="27" t="s">
@@ -884,25 +934,25 @@
       <c r="I15" s="28"/>
       <c r="J15" s="28"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:10">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" ht="9.75" customHeight="1" spans="1:4">
+    <row r="17" spans="1:11" ht="9.75" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:11">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" ht="12.75" customHeight="1" spans="1:10">
+    <row r="19" spans="1:11" ht="12.75" customHeight="1">
       <c r="A19" s="29" t="s">
         <v>24</v>
       </c>
@@ -916,7 +966,7 @@
       <c r="I19" s="29"/>
       <c r="J19" s="29"/>
     </row>
-    <row r="20" ht="23" customHeight="1" spans="1:10">
+    <row r="20" spans="1:11" ht="23.1" customHeight="1">
       <c r="A20" s="29"/>
       <c r="B20" s="29"/>
       <c r="C20" s="29"/>
@@ -928,11 +978,11 @@
       <c r="I20" s="29"/>
       <c r="J20" s="29"/>
     </row>
-    <row r="22" ht="12.75" customHeight="1"/>
-    <row r="23" ht="12.75" customHeight="1"/>
-    <row r="24" ht="12.75" customHeight="1"/>
-    <row r="25" ht="24" customHeight="1"/>
-    <row r="26" s="1" customFormat="1" ht="26.25" customHeight="1" spans="1:11">
+    <row r="22" spans="1:11" ht="12.75" customHeight="1"/>
+    <row r="23" spans="1:11" ht="12.75" customHeight="1"/>
+    <row r="24" spans="1:11" ht="12.75" customHeight="1"/>
+    <row r="25" spans="1:11" ht="24" customHeight="1"/>
+    <row r="26" spans="1:11" s="1" customFormat="1" ht="26.25" customHeight="1">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -945,7 +995,7 @@
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
     </row>
-    <row r="27" s="1" customFormat="1" ht="27" customHeight="1" spans="1:11">
+    <row r="27" spans="1:11" s="1" customFormat="1" ht="27" customHeight="1">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -958,7 +1008,7 @@
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
     </row>
-    <row r="28" s="1" customFormat="1" ht="27" customHeight="1" spans="1:11">
+    <row r="28" spans="1:11" s="1" customFormat="1" ht="27" customHeight="1">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -971,7 +1021,7 @@
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
     </row>
-    <row r="29" s="1" customFormat="1" ht="27" customHeight="1" spans="1:11">
+    <row r="29" spans="1:11" s="1" customFormat="1" ht="27" customHeight="1">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -984,7 +1034,7 @@
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
     </row>
-    <row r="30" s="1" customFormat="1" ht="27" customHeight="1" spans="1:11">
+    <row r="30" spans="1:11" s="1" customFormat="1" ht="27" customHeight="1">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -997,7 +1047,7 @@
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
     </row>
-    <row r="31" s="1" customFormat="1" ht="27" customHeight="1" spans="1:11">
+    <row r="31" spans="1:11" s="1" customFormat="1" ht="27" customHeight="1">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1010,7 +1060,7 @@
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
     </row>
-    <row r="32" s="1" customFormat="1" ht="27.75" customHeight="1" spans="1:11">
+    <row r="32" spans="1:11" s="1" customFormat="1" ht="27.75" customHeight="1">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1023,7 +1073,7 @@
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
     </row>
-    <row r="33" s="1" customFormat="1" ht="27" customHeight="1" spans="1:11">
+    <row r="33" spans="1:11" s="1" customFormat="1" ht="27" customHeight="1">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1036,8 +1086,8 @@
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
     </row>
-    <row r="34" ht="10.5" customHeight="1"/>
-    <row r="36" s="2" customFormat="1" spans="1:11">
+    <row r="34" spans="1:11" ht="10.5" customHeight="1"/>
+    <row r="36" spans="1:11" s="2" customFormat="1">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -1050,10 +1100,16 @@
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
     </row>
-    <row r="40" ht="12.75" customHeight="1"/>
-    <row r="41" ht="15" customHeight="1"/>
+    <row r="40" spans="1:11" ht="12.75" customHeight="1"/>
+    <row r="41" spans="1:11" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="A19:J20"/>
+    <mergeCell ref="C1:J3"/>
+    <mergeCell ref="B8:J9"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B13:D13"/>
@@ -1061,17 +1117,10 @@
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="H14:J14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="H15:J15"/>
-    <mergeCell ref="A19:J20"/>
-    <mergeCell ref="C1:J3"/>
-    <mergeCell ref="B8:J9"/>
   </mergeCells>
   <pageMargins left="0.2" right="0.2" top="0" bottom="0" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Allow Air & Hang Roi add trucking fee
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/PhieuChiTemplate.xlsx
+++ b/src/main/resources/ExportTemplate/PhieuChiTemplate.xlsx
@@ -10,7 +10,6 @@
     <sheet name="PHIEU  CHI " sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -249,6 +248,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -260,24 +277,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -303,8 +302,8 @@
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1857375</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
@@ -703,51 +702,51 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="28" style="3" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" style="3" customWidth="1"/>
     <col min="2" max="2" width="6.5703125" style="3" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="3"/>
-    <col min="4" max="4" width="10.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" style="3" customWidth="1"/>
     <col min="5" max="5" width="4.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="3" customWidth="1"/>
     <col min="7" max="7" width="6.5703125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="3"/>
+    <col min="8" max="8" width="7.140625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" style="3" customWidth="1"/>
     <col min="10" max="10" width="11.85546875" style="3" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12.75" customHeight="1">
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" spans="1:10" ht="12.75" customHeight="1">
       <c r="B2" s="4"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
     </row>
     <row r="3" spans="1:10" ht="12.75" customHeight="1">
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
     </row>
     <row r="4" spans="1:10" ht="24" customHeight="1">
       <c r="C4" s="5" t="s">
@@ -780,10 +779,10 @@
       <c r="H5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="23" t="s">
+      <c r="I5" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="23"/>
+      <c r="J5" s="29"/>
     </row>
     <row r="6" spans="1:10" s="1" customFormat="1" ht="27" customHeight="1">
       <c r="A6" s="5" t="s">
@@ -817,44 +816,44 @@
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
     </row>
     <row r="9" spans="1:10" s="1" customFormat="1" ht="27" customHeight="1">
       <c r="A9" s="10"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
     </row>
     <row r="10" spans="1:10" s="1" customFormat="1" ht="27" customHeight="1">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
       <c r="J10" s="12"/>
     </row>
     <row r="11" spans="1:10" s="1" customFormat="1" ht="27.75" customHeight="1">
@@ -887,52 +886,52 @@
     </row>
     <row r="13" spans="1:10" ht="28.5" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25" t="s">
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="26" t="s">
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
     </row>
     <row r="15" spans="1:10" s="2" customFormat="1">
       <c r="A15" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="28" t="s">
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28" t="s">
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="1"/>
@@ -953,30 +952,30 @@
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:11" ht="12.75" customHeight="1">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="29"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="25"/>
     </row>
     <row r="20" spans="1:11" ht="23.1" customHeight="1">
-      <c r="A20" s="29"/>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
+      <c r="A20" s="25"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
     </row>
     <row r="22" spans="1:11" ht="12.75" customHeight="1"/>
     <row r="23" spans="1:11" ht="12.75" customHeight="1"/>
@@ -1119,8 +1118,8 @@
     <mergeCell ref="H14:J14"/>
   </mergeCells>
   <pageMargins left="0.2" right="0.2" top="0" bottom="0" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>